<commit_message>
new naming system for aux vars
</commit_message>
<xml_diff>
--- a/JoeHasell/Copy_of_Michalis_work/control_stubs.xlsx
+++ b/JoeHasell/Copy_of_Michalis_work/control_stubs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joehasell/Documents/OWID/notebooks/JoeHasell/Copy_of_Michalis_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0BD390F-005B-734A-A96A-A9C875EA0B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{40530701-4298-8144-8977-3456DD78A055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="3520" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{376489E3-129A-9E4B-A657-B41146175634}"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{376489E3-129A-9E4B-A657-B41146175634}"/>
   </bookViews>
   <sheets>
     <sheet name="control_stubs" sheetId="1" r:id="rId1"/>
     <sheet name="abs_povline" sheetId="2" r:id="rId2"/>
+    <sheet name="welfare" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="83">
   <si>
     <t>Aux</t>
   </si>
@@ -77,22 +78,7 @@
     <t>abs_povline_currency, welfare</t>
   </si>
   <si>
-    <t>headcount_ratio_[abs_povline_currency]</t>
-  </si>
-  <si>
-    <t>[welfare]</t>
-  </si>
-  <si>
     <t>Share in poverty</t>
-  </si>
-  <si>
-    <t>$[abs_povline_currency] a day</t>
-  </si>
-  <si>
-    <t>$[abs_povline_currency] a day - share of population below poverty line</t>
-  </si>
-  <si>
-    <t>Poverty: Share of population living on less than $[abs_povline_currency] a day</t>
   </si>
   <si>
     <t>This data is adjusted for differences in the cost of living between countries and for inflation.</t>
@@ -107,28 +93,10 @@
     <t>%</t>
   </si>
   <si>
-    <t>headcount_[abs_povline_currency]</t>
-  </si>
-  <si>
     <t>Number of people in poverty</t>
   </si>
   <si>
-    <t>$[abs_povline_currency] a day - total number of people below poverty line</t>
-  </si>
-  <si>
-    <t>Poverty: Number of people living on less than $[abs_povline_currency] a day</t>
-  </si>
-  <si>
-    <t>avg_shortfall_[abs_povline_currency]</t>
-  </si>
-  <si>
     <t>Average shortfall below poverty line ($ per day)</t>
-  </si>
-  <si>
-    <t>$[abs_povline_currency] a day - shortfall per person in poverty ($ per day)</t>
-  </si>
-  <si>
-    <t>Depth of poverty: Average daily shortfall of [welfare] below $[abs_povline_currency] a day</t>
   </si>
   <si>
     <t>The average shortfall from the poverty line per day (averaged across the population in poverty).</t>
@@ -143,46 +111,19 @@
     <t>$</t>
   </si>
   <si>
-    <t>income_gap_ratio_[abs_povline_currency]</t>
-  </si>
-  <si>
     <t>Average shortfall below poverty line (% of poverty line)</t>
-  </si>
-  <si>
-    <t>$[abs_povline_currency] a day - shortfall per person in poverty (% of poverty line)</t>
-  </si>
-  <si>
-    <t>Depth of poverty: Average percentage shortfall of [welfare] below $[abs_povline_currency] a day</t>
   </si>
   <si>
     <t>This metric is sometimes called the 'income gap ratio'. It measures the average shortfall from the poverty line (averaged across the population in poverty) expressed as a share of the poverty line.</t>
   </si>
   <si>
-    <t>total_shortall_daily_[abs_povline_currency]</t>
-  </si>
-  <si>
     <t>Total shortfall below poverty line</t>
-  </si>
-  <si>
-    <t>$[abs_povline_currency] a day - total shortfall per day</t>
-  </si>
-  <si>
-    <t>Total daily shortfall of [welfare] below $[abs_povline_currency] a day</t>
   </si>
   <si>
     <t>The total shortfall from the poverty line per day (summed across the population in poverty).</t>
   </si>
   <si>
-    <t>poverty_gap_index_[abs_povline_currency]</t>
-  </si>
-  <si>
     <t>Poverty gap index</t>
-  </si>
-  <si>
-    <t>$[abs_povline_currency] a day - Poverty gap index</t>
-  </si>
-  <si>
-    <t>Poverty gap index at $[abs_povline_currency] a day.</t>
   </si>
   <si>
     <t>The poverty gap index is the average shortfall from the poverty line, averaged across the whole population where the non-poor are counted as having zero shortfall. It is expressed as a percentage of the poverty line.</t>
@@ -249,6 +190,102 @@
   </si>
   <si>
     <t>40_00</t>
+  </si>
+  <si>
+    <t>abs_povline, welfare</t>
+  </si>
+  <si>
+    <t>incomes or consumption</t>
+  </si>
+  <si>
+    <t>incomes</t>
+  </si>
+  <si>
+    <t>consumption</t>
+  </si>
+  <si>
+    <t>table_names</t>
+  </si>
+  <si>
+    <t>inc_or_cons</t>
+  </si>
+  <si>
+    <t>inc</t>
+  </si>
+  <si>
+    <t>cons</t>
+  </si>
+  <si>
+    <t>radio_option</t>
+  </si>
+  <si>
+    <t>Incomes only</t>
+  </si>
+  <si>
+    <t>Either income or consumption</t>
+  </si>
+  <si>
+    <t>Consumption only</t>
+  </si>
+  <si>
+    <t>$[abs_povline$text] a day</t>
+  </si>
+  <si>
+    <t>headcount_ratio_[abs_povline$slug_suffix]</t>
+  </si>
+  <si>
+    <t>headcount_[abs_povline$slug_suffix]</t>
+  </si>
+  <si>
+    <t>avg_shortfall_[abs_povline$slug_suffix]</t>
+  </si>
+  <si>
+    <t>income_gap_ratio_[abs_povline$slug_suffix]</t>
+  </si>
+  <si>
+    <t>total_shortall_daily_[abs_povline$slug_suffix]</t>
+  </si>
+  <si>
+    <t>poverty_gap_index_[abs_povline$slug_suffix]</t>
+  </si>
+  <si>
+    <t>$[abs_povline$text]a day - share of population below poverty line</t>
+  </si>
+  <si>
+    <t>$[abs_povline$text] a day - total number of people below poverty line</t>
+  </si>
+  <si>
+    <t>$[abs_povline$text] a day - shortfall per person in poverty ($ per day)</t>
+  </si>
+  <si>
+    <t>$[abs_povline$text] a day - shortfall per person in poverty (% of poverty line)</t>
+  </si>
+  <si>
+    <t>$[abs_povline$text] a day - total shortfall per day</t>
+  </si>
+  <si>
+    <t>$[abs_povline$text] a day - Poverty gap index</t>
+  </si>
+  <si>
+    <t>Poverty: Share of population living on less than $[abs_povline$text] a day</t>
+  </si>
+  <si>
+    <t>Poverty: Number of people living on less than $[abs_povline$text] a day</t>
+  </si>
+  <si>
+    <t>Poverty gap index at $[abs_povline$text] a day.</t>
+  </si>
+  <si>
+    <t>[welfare$table_names]</t>
+  </si>
+  <si>
+    <t>Depth of poverty: Average percentage shortfall of [welfare$text] below $[abs_povline$text] a day</t>
+  </si>
+  <si>
+    <t>Total daily shortfall of [welfare$text] below $[abs_povline$text] a day</t>
+  </si>
+  <si>
+    <t>Depth of poverty: Average daily shortfall of [welfare$text] below $[abs_povline$text] a day</t>
   </si>
 </sst>
 </file>
@@ -640,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD181DE-64E9-1643-81E5-FFA509608C40}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,40 +750,40 @@
     </row>
     <row r="2" spans="1:32" ht="43" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -774,31 +811,31 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -828,37 +865,37 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="K4" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -886,37 +923,37 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="K5" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -944,37 +981,37 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="K6" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1002,37 +1039,37 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="K7" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -34826,7 +34863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C948085-E7B3-7541-81A4-1BE55D2FDA70}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -34834,21 +34871,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -34856,10 +34893,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>1.9</v>
@@ -34867,10 +34904,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>3.2</v>
@@ -34878,10 +34915,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>5.5</v>
@@ -34889,10 +34926,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -34900,10 +34937,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -34911,10 +34948,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -34922,10 +34959,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C9">
         <v>30</v>
@@ -34933,10 +34970,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -34949,4 +34986,66 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9387555A-3082-954B-83C9-D46BCE0DA8B3}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>